<commit_message>
valid test data for new user creation
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lokes\Downloads\Framework_Code_With_Script (1)\HybridFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ABC46A-ADB3-43AA-A1A0-7F2174C56771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48490E28-FCFC-4127-848D-BF71CBE07686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
     <t>Male</t>
   </si>
   <si>
-    <t>lokeshkumar.d2000@gmail.com</t>
+    <t>lokeshkumar.automation@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>